<commit_message>
update: Adding GUI(in progress)
</commit_message>
<xml_diff>
--- a/Destroyer/Destroyer_2021-08-12.xlsx
+++ b/Destroyer/Destroyer_2021-08-12.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>잔트</t>
   </si>
@@ -115,9 +115,6 @@
     <t>오거돈</t>
   </si>
   <si>
-    <t>앰살</t>
-  </si>
-  <si>
     <t>이거안뜨면접어요</t>
   </si>
   <si>
@@ -167,9 +164,6 @@
   </si>
   <si>
     <t>언죠비카이</t>
-  </si>
-  <si>
-    <t>되겐냐</t>
   </si>
   <si>
     <t>폴블랑코</t>
@@ -650,7 +644,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A94"/>
+  <dimension ref="A1:A92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1116,16 +1110,6 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="s">
-        <v>92</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>